<commit_message>
reduce amnt opened txtr | Fixed hasValues
</commit_message>
<xml_diff>
--- a/experiment/RUN_ME/stimuli/trial_lists/practice_trials.xlsx
+++ b/experiment/RUN_ME/stimuli/trial_lists/practice_trials.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\university\mudrick_lab\subliminal_priming_w_motion_capture\experiment\RUN_ME\stimuli\trial_lists\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{880CD6D3-1D5D-4634-B3DF-3C5D36826E51}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6390904C-9F34-4DC0-BE95-881C42AA2574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="3930" windowWidth="18900" windowHeight="11055" xr2:uid="{C9482004-E1A8-40D2-8095-0843D42A0E65}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{C9482004-E1A8-40D2-8095-0843D42A0E65}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -684,7 +684,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABCEE904-871D-4D8E-8A05-FC58730D7D77}">
   <dimension ref="A1:BF41"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -701,7 +703,7 @@
     <col min="11" max="11" width="8.875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="5.5" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="14" max="16" width="6.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="16" width="9.75" customWidth="1"/>
     <col min="17" max="17" width="10.125" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="14" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="13.125" bestFit="1" customWidth="1"/>
@@ -948,13 +950,13 @@
         <v>1</v>
       </c>
       <c r="N2">
-        <v>54</v>
+        <v>25</v>
       </c>
       <c r="O2">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="P2">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="Q2">
         <v>1</v>
@@ -1016,13 +1018,13 @@
         <v>0</v>
       </c>
       <c r="N3">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="O3">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="P3">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="Q3">
         <v>1</v>
@@ -1084,13 +1086,13 @@
         <v>1</v>
       </c>
       <c r="N4">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="O4">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="P4">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="Q4">
         <v>1</v>
@@ -1152,13 +1154,13 @@
         <v>0</v>
       </c>
       <c r="N5">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="O5">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="P5">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="Q5">
         <v>1</v>
@@ -1220,13 +1222,13 @@
         <v>1</v>
       </c>
       <c r="N6">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="O6">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="P6">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="Q6">
         <v>1</v>
@@ -1288,13 +1290,13 @@
         <v>1</v>
       </c>
       <c r="N7">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="O7">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="P7">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="Q7">
         <v>1</v>
@@ -1356,13 +1358,13 @@
         <v>0</v>
       </c>
       <c r="N8">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="O8">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="P8">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="Q8">
         <v>1</v>
@@ -1424,13 +1426,13 @@
         <v>1</v>
       </c>
       <c r="N9">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="O9">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="P9">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="Q9">
         <v>1</v>
@@ -1492,13 +1494,13 @@
         <v>0</v>
       </c>
       <c r="N10">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="O10">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="P10">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="Q10">
         <v>1</v>
@@ -1560,13 +1562,13 @@
         <v>1</v>
       </c>
       <c r="N11">
-        <v>30</v>
+        <v>1</v>
       </c>
       <c r="O11">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="P11">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="Q11">
         <v>1</v>
@@ -1628,13 +1630,13 @@
         <v>1</v>
       </c>
       <c r="N12">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="O12">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="P12">
-        <v>73</v>
+        <v>44</v>
       </c>
       <c r="Q12">
         <v>1</v>
@@ -1696,13 +1698,13 @@
         <v>1</v>
       </c>
       <c r="N13">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="O13">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="P13">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="Q13">
         <v>1</v>
@@ -1764,13 +1766,13 @@
         <v>1</v>
       </c>
       <c r="N14">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O14">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="P14">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="Q14">
         <v>1</v>
@@ -1832,13 +1834,13 @@
         <v>0</v>
       </c>
       <c r="N15">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="O15">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="P15">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="Q15">
         <v>1</v>
@@ -1900,13 +1902,13 @@
         <v>0</v>
       </c>
       <c r="N16">
-        <v>62</v>
+        <v>33</v>
       </c>
       <c r="O16">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="P16">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="Q16">
         <v>1</v>
@@ -1968,13 +1970,13 @@
         <v>1</v>
       </c>
       <c r="N17">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="O17">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="P17">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="Q17">
         <v>1</v>
@@ -2036,13 +2038,13 @@
         <v>1</v>
       </c>
       <c r="N18">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="O18">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="P18">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="Q18">
         <v>1</v>
@@ -2104,13 +2106,13 @@
         <v>0</v>
       </c>
       <c r="N19">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="O19">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="P19">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="Q19">
         <v>1</v>
@@ -2172,13 +2174,13 @@
         <v>1</v>
       </c>
       <c r="N20">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="O20">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="P20">
-        <v>45</v>
+        <v>16</v>
       </c>
       <c r="Q20">
         <v>1</v>
@@ -2240,13 +2242,13 @@
         <v>1</v>
       </c>
       <c r="N21">
-        <v>84</v>
+        <v>55</v>
       </c>
       <c r="O21">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="P21">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="Q21">
         <v>1</v>
@@ -2308,13 +2310,13 @@
         <v>1</v>
       </c>
       <c r="N22">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="O22">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="P22">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="Q22">
         <v>1</v>
@@ -2376,13 +2378,13 @@
         <v>0</v>
       </c>
       <c r="N23">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="O23">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="P23">
-        <v>38</v>
+        <v>9</v>
       </c>
       <c r="Q23">
         <v>1</v>
@@ -2444,13 +2446,13 @@
         <v>0</v>
       </c>
       <c r="N24">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="O24">
-        <v>61</v>
+        <v>32</v>
       </c>
       <c r="P24">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="Q24">
         <v>1</v>
@@ -2512,13 +2514,13 @@
         <v>0</v>
       </c>
       <c r="N25">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="O25">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="P25">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="Q25">
         <v>1</v>
@@ -2580,13 +2582,13 @@
         <v>0</v>
       </c>
       <c r="N26">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="O26">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="P26">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="Q26">
         <v>1</v>
@@ -2648,13 +2650,13 @@
         <v>1</v>
       </c>
       <c r="N27">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="O27">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="P27">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="Q27">
         <v>1</v>
@@ -2716,13 +2718,13 @@
         <v>0</v>
       </c>
       <c r="N28">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="O28">
-        <v>64</v>
+        <v>35</v>
       </c>
       <c r="P28">
-        <v>87</v>
+        <v>58</v>
       </c>
       <c r="Q28">
         <v>1</v>
@@ -2784,13 +2786,13 @@
         <v>0</v>
       </c>
       <c r="N29">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="O29">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="P29">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="Q29">
         <v>1</v>
@@ -2852,13 +2854,13 @@
         <v>1</v>
       </c>
       <c r="N30">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="O30">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="P30">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="Q30">
         <v>1</v>
@@ -2920,13 +2922,13 @@
         <v>1</v>
       </c>
       <c r="N31">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="O31">
-        <v>63</v>
+        <v>34</v>
       </c>
       <c r="P31">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="Q31">
         <v>1</v>
@@ -2988,13 +2990,13 @@
         <v>1</v>
       </c>
       <c r="N32">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="O32">
-        <v>82</v>
+        <v>53</v>
       </c>
       <c r="P32">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="Q32">
         <v>1</v>
@@ -3056,13 +3058,13 @@
         <v>0</v>
       </c>
       <c r="N33">
-        <v>85</v>
+        <v>56</v>
       </c>
       <c r="O33">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="P33">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="Q33">
         <v>1</v>
@@ -3124,13 +3126,13 @@
         <v>1</v>
       </c>
       <c r="N34">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="O34">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="P34">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="Q34">
         <v>1</v>
@@ -3192,13 +3194,13 @@
         <v>0</v>
       </c>
       <c r="N35">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="O35">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="P35">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="Q35">
         <v>1</v>
@@ -3260,13 +3262,13 @@
         <v>1</v>
       </c>
       <c r="N36">
-        <v>66</v>
+        <v>37</v>
       </c>
       <c r="O36">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="P36">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="Q36">
         <v>1</v>
@@ -3328,13 +3330,13 @@
         <v>0</v>
       </c>
       <c r="N37">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="O37">
-        <v>32</v>
+        <v>3</v>
       </c>
       <c r="P37">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="Q37">
         <v>1</v>
@@ -3396,13 +3398,13 @@
         <v>0</v>
       </c>
       <c r="N38">
-        <v>68</v>
+        <v>39</v>
       </c>
       <c r="O38">
-        <v>76</v>
+        <v>47</v>
       </c>
       <c r="P38">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="Q38">
         <v>1</v>
@@ -3464,13 +3466,13 @@
         <v>0</v>
       </c>
       <c r="N39">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="O39">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="P39">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="Q39">
         <v>1</v>
@@ -3532,13 +3534,13 @@
         <v>0</v>
       </c>
       <c r="N40">
-        <v>86</v>
+        <v>57</v>
       </c>
       <c r="O40">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="P40">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="Q40">
         <v>1</v>
@@ -3600,13 +3602,13 @@
         <v>0</v>
       </c>
       <c r="N41">
-        <v>88</v>
+        <v>59</v>
       </c>
       <c r="O41">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="P41">
-        <v>31</v>
+        <v>2</v>
       </c>
       <c r="Q41">
         <v>1</v>

</xml_diff>